<commit_message>
Advent2016: Added equasion that gives the number of moves necessary in xlsx file for Day11
</commit_message>
<xml_diff>
--- a/Advent2016/Day/D11.xlsx
+++ b/Advent2016/Day/D11.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="24">
   <si>
     <t>E</t>
   </si>
@@ -86,10 +86,16 @@
     <t>17 moves up to this state, collecting remaining Chips is extra 19 which totals up to 36.</t>
   </si>
   <si>
-    <t>https://www.reddit.com/r/adventofcode/comments/5hoia9/2016_day_11_solutions/db1ygvm/</t>
+    <t xml:space="preserve">It works if the generator and chip are in pairs. However. In my puzzle, I was one move away from paired elements, which is translated as an offset of 4 - dunno why. </t>
   </si>
   <si>
-    <t xml:space="preserve">It works if the generator and chip are in pairs. However. In my puzzle, I was one move away from paired elements, which is translated as an offset of 4 - dunno why. </t>
+    <t>Equasion</t>
+  </si>
+  <si>
+    <t>n - floor</t>
+  </si>
+  <si>
+    <t>I - number of items on corresponding n'th floor</t>
   </si>
 </sst>
 </file>
@@ -205,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -225,6 +231,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,6 +249,82 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99249E0F-5ECC-49FB-931D-2FD6197B70E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1628775" y="17726025"/>
+          <a:ext cx="1400175" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,7 +627,7 @@
   <dimension ref="A1:Q104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="Q98" sqref="Q98"/>
+      <selection activeCell="M96" sqref="M96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,17 +2205,30 @@
         <v>19</v>
       </c>
     </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M94" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M95" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M96" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="97" spans="13:17" x14ac:dyDescent="0.25">
-      <c r="M97" t="s">
-        <v>20</v>
-      </c>
+      <c r="M97" s="13"/>
     </row>
     <row r="98" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M98" t="s">
         <v>13</v>
       </c>
       <c r="Q98" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="13:17" x14ac:dyDescent="0.25">
@@ -2597,5 +2695,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>